<commit_message>
Updated with new scraping round
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -164,18 +164,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="\+#,##0%;\-#,##0%"/>
-    <numFmt numFmtId="169" formatCode="0.0%"/>
-    <numFmt numFmtId="170" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="\+#,##0%;\-#,##0%"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -208,12 +201,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -242,78 +241,81 @@
   </borders>
   <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -678,7 +680,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection sqref="A1:F6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -693,122 +695,122 @@
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1">
       <c r="A1" s="6"/>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>1135</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10">
-        <v>12775</v>
-      </c>
-      <c r="E2" s="11" t="s">
+      <c r="D2" s="16">
+        <v>12754</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <f>D2/B2-1</f>
-        <v>10.255506607929515</v>
+        <v>10.237004405286344</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>96</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="12">
         <f>B3/B2</f>
         <v>8.4581497797356825E-2</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <v>2842</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="12">
         <f>D3/D2</f>
-        <v>0.22246575342465755</v>
-      </c>
-      <c r="F3" s="12">
+        <v>0.22283205268935236</v>
+      </c>
+      <c r="F3" s="11">
         <f>D3/B3-1</f>
         <v>28.604166666666668</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>58</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="9">
         <v>620</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>1</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <f>B5/B2</f>
         <v>8.81057268722467E-4</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="9">
         <v>40</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="12">
         <f>D5/D2</f>
-        <v>3.1311154598825833E-3</v>
-      </c>
-      <c r="F5" s="12">
+        <v>3.1362709738121373E-3</v>
+      </c>
+      <c r="F5" s="11">
         <f>D5/B5-1</f>
         <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="9">
         <v>35</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>3</v>
       </c>
     </row>
@@ -832,7 +834,7 @@
       </c>
       <c r="D9" s="3">
         <f>D2-D3</f>
-        <v>9933</v>
+        <v>9912</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -864,13 +866,13 @@
     <row r="13" spans="1:6">
       <c r="B13" s="5">
         <f>POWER(F2+1,1/22)</f>
-        <v>1.1163215800284221</v>
+        <v>1.1162381031912056</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="5">
         <f>POWER(B13,22)-1</f>
-        <v>10.255506607929487</v>
+        <v>10.237004405286324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished updating with last night's scraping round
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -201,18 +201,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -239,8 +233,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -315,11 +343,11 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="63">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -334,6 +362,23 @@
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -348,6 +393,23 @@
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -680,7 +742,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -739,16 +801,16 @@
         <f>B3/B2</f>
         <v>8.4581497797356825E-2</v>
       </c>
-      <c r="D3" s="9">
-        <v>2842</v>
+      <c r="D3" s="16">
+        <v>2852</v>
       </c>
       <c r="E3" s="12">
         <f>D3/D2</f>
-        <v>0.22283205268935236</v>
+        <v>0.2236161204328054</v>
       </c>
       <c r="F3" s="11">
         <f>D3/B3-1</f>
-        <v>28.604166666666668</v>
+        <v>28.708333333333332</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -761,8 +823,8 @@
       <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9">
-        <v>620</v>
+      <c r="D4" s="16">
+        <v>632</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>3</v>
@@ -782,16 +844,16 @@
         <f>B5/B2</f>
         <v>8.81057268722467E-4</v>
       </c>
-      <c r="D5" s="9">
-        <v>40</v>
+      <c r="D5" s="16">
+        <v>38</v>
       </c>
       <c r="E5" s="12">
         <f>D5/D2</f>
-        <v>3.1362709738121373E-3</v>
+        <v>2.9794574251215305E-3</v>
       </c>
       <c r="F5" s="11">
         <f>D5/B5-1</f>
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -804,8 +866,8 @@
       <c r="C6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9">
-        <v>35</v>
+      <c r="D6" s="16">
+        <v>16</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>3</v>
@@ -834,7 +896,7 @@
       </c>
       <c r="D9" s="3">
         <f>D2-D3</f>
-        <v>9912</v>
+        <v>9902</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -847,7 +909,7 @@
       </c>
       <c r="D10" s="3">
         <f>D3-D5</f>
-        <v>2802</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -860,7 +922,7 @@
       </c>
       <c r="D11" s="3">
         <f>D5</f>
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">

</xml_diff>

<commit_message>
Updated vs latest scrape
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="520" yWindow="0" windowWidth="23180" windowHeight="17240" tabRatio="500"/>
+    <workbookView xWindow="5340" yWindow="0" windowWidth="23180" windowHeight="17240" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>May 2012</t>
   </si>
@@ -33,6 +33,33 @@
     <t>-</t>
   </si>
   <si>
+    <r>
+      <t>No. of products or services containing the word "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" in the description</t>
+    </r>
+  </si>
+  <si>
     <t>Non-data products and services</t>
   </si>
   <si>
@@ -43,9 +70,6 @@
   </si>
   <si>
     <t>Total number of products or services</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>No. of suppliers providing the above</t>
@@ -76,36 +100,6 @@
       </rPr>
       <t>" in the description and that appear to be genuine users of open data or having a proposition strongly centred around open data</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>No. of products or services containing the word "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>data</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="128"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>" in the description (1)</t>
-    </r>
-  </si>
-  <si>
-    <t>(1) We found cases in which CloudStore's full-text search did not return some of the expected results, e.g. searching for "data" did not list some of the services that refer to "open data" in their description. We used workarounds wherever possible to avoid this issue to influence the reliability of the results.</t>
   </si>
 </sst>
 </file>
@@ -258,7 +252,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -310,24 +304,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -729,10 +705,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -761,7 +737,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="7">
         <v>1135</v>
@@ -782,7 +758,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="16" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B3" s="7">
         <v>96</v>
@@ -791,16 +767,16 @@
         <f>B3/B2</f>
         <v>8.4581497797356825E-2</v>
       </c>
-      <c r="D3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="10" t="e">
+      <c r="D3" s="13">
+        <v>3116</v>
+      </c>
+      <c r="E3" s="10">
         <f>D3/D2</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="F3" s="9" t="e">
+        <v>0.2443921568627451</v>
+      </c>
+      <c r="F3" s="9">
         <f>D3/B3-1</f>
-        <v>#VALUE!</v>
+        <v>31.458333333333336</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -813,8 +789,8 @@
       <c r="C4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>8</v>
+      <c r="D4" s="13">
+        <v>656</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>3</v>
@@ -866,98 +842,79 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="6" customHeight="1">
+    <row r="7" spans="1:6" s="17" customFormat="1" ht="28" customHeight="1">
       <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" ht="28" customHeight="1">
-      <c r="A8" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-    </row>
-    <row r="9" spans="1:6" s="17" customFormat="1" ht="28" customHeight="1">
-      <c r="A9" s="24"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="B10" s="3" t="str">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="3" t="str">
         <f>B1</f>
         <v>May 2012</v>
       </c>
-      <c r="D10" s="3" t="str">
+      <c r="D8" s="3" t="str">
         <f>D1</f>
         <v>Mar 2014</v>
       </c>
     </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3">
+        <f>B2-B3</f>
+        <v>1039</v>
+      </c>
+      <c r="D9" s="3">
+        <f>D2-D3</f>
+        <v>9634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <f>B3-B5</f>
+        <v>95</v>
+      </c>
+      <c r="D10" s="3">
+        <f>D3-D5</f>
+        <v>3094</v>
+      </c>
+    </row>
     <row r="11" spans="1:6">
       <c r="A11" s="17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3">
-        <f>B2-B3</f>
-        <v>1039</v>
-      </c>
-      <c r="D11" s="3" t="e">
-        <f>D2-D3</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="3">
-        <f>B3-B5</f>
-        <v>95</v>
-      </c>
-      <c r="D12" s="3" t="e">
-        <f>D3-D5</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3">
         <f>B5</f>
         <v>1</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D11" s="3">
         <f>D5</f>
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="B15" s="5">
+    <row r="13" spans="1:6">
+      <c r="B13" s="5">
         <f>POWER(F2+1,1/22)</f>
         <v>1.1162221879671452</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="5">
-        <f>POWER(B15,22)-1</f>
+    <row r="14" spans="1:6">
+      <c r="B14" s="5">
+        <f>POWER(B13,22)-1</f>
         <v>10.233480176211474</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="A8:F8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>